<commit_message>
Tabla de resultados actualizado
</commit_message>
<xml_diff>
--- a/report/Tabla de resultados.xlsx
+++ b/report/Tabla de resultados.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="97">
   <si>
     <t>Logit</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Ocacional 0 / Permanente 1</t>
   </si>
   <si>
-    <t>Odds</t>
-  </si>
-  <si>
-    <t>Ratio</t>
-  </si>
-  <si>
     <t>Grupo edad (0-17)</t>
   </si>
   <si>
@@ -154,13 +148,175 @@
   </si>
   <si>
     <t>(0.027)</t>
+  </si>
+  <si>
+    <t>-1.157***</t>
+  </si>
+  <si>
+    <t>-0.207***</t>
+  </si>
+  <si>
+    <t>-0.709***</t>
+  </si>
+  <si>
+    <t>-0.214***</t>
+  </si>
+  <si>
+    <t>-1.067***</t>
+  </si>
+  <si>
+    <t>-0.188***</t>
+  </si>
+  <si>
+    <t>-0.653***</t>
+  </si>
+  <si>
+    <t>-0.195***</t>
+  </si>
+  <si>
+    <t>-0.724***</t>
+  </si>
+  <si>
+    <t>-0.12***</t>
+  </si>
+  <si>
+    <t>-0.127***</t>
+  </si>
+  <si>
+    <t>0.273***</t>
+  </si>
+  <si>
+    <t>0.057***</t>
+  </si>
+  <si>
+    <t>0.165***</t>
+  </si>
+  <si>
+    <t>0.105***</t>
+  </si>
+  <si>
+    <t>0.021***</t>
+  </si>
+  <si>
+    <t>0.064***</t>
+  </si>
+  <si>
+    <t>-0.655***</t>
+  </si>
+  <si>
+    <t>-0.141***</t>
+  </si>
+  <si>
+    <t>-0.399***</t>
+  </si>
+  <si>
+    <t>-0.14***</t>
+  </si>
+  <si>
+    <t>-1233***</t>
+  </si>
+  <si>
+    <t>-0.269***</t>
+  </si>
+  <si>
+    <t>-0.755***</t>
+  </si>
+  <si>
+    <t>0.453***</t>
+  </si>
+  <si>
+    <t>0.084***</t>
+  </si>
+  <si>
+    <t>0.272***</t>
+  </si>
+  <si>
+    <t>-1.701***</t>
+  </si>
+  <si>
+    <t>-0.394***</t>
+  </si>
+  <si>
+    <t>-1.053***</t>
+  </si>
+  <si>
+    <t>-0.395***</t>
+  </si>
+  <si>
+    <t>-3.995***</t>
+  </si>
+  <si>
+    <t>-0.638***</t>
+  </si>
+  <si>
+    <t>-2.236***</t>
+  </si>
+  <si>
+    <t>-0.636***</t>
+  </si>
+  <si>
+    <t>-3.028***</t>
+  </si>
+  <si>
+    <t>-0.581***</t>
+  </si>
+  <si>
+    <t>-1.782***</t>
+  </si>
+  <si>
+    <t>-0.58***</t>
+  </si>
+  <si>
+    <t>-3.507***</t>
+  </si>
+  <si>
+    <t>-0.615***</t>
+  </si>
+  <si>
+    <t>-2.023***</t>
+  </si>
+  <si>
+    <t>-0.614***</t>
+  </si>
+  <si>
+    <t>-0.187***</t>
+  </si>
+  <si>
+    <t>-0.039***</t>
+  </si>
+  <si>
+    <t>-0.116***</t>
+  </si>
+  <si>
+    <t>-0.04***</t>
+  </si>
+  <si>
+    <t>-1.046***</t>
+  </si>
+  <si>
+    <t>-0.234***</t>
+  </si>
+  <si>
+    <t>-0.658***</t>
+  </si>
+  <si>
+    <t>-0.239***</t>
+  </si>
+  <si>
+    <t>-0.449***</t>
+  </si>
+  <si>
+    <t>* p&lt;0.05, ** p&lt;0.01, *** p&lt;0.001</t>
+  </si>
+  <si>
+    <t>dy/dx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +342,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Garamond"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -214,7 +377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -356,37 +519,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -420,6 +581,42 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,7 +835,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -653,605 +850,615 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="30"/>
+    </row>
+    <row r="4" spans="1:5" ht="14.5">
+      <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="1:5" ht="14.5">
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="14.5">
-      <c r="A4" s="11" t="s">
+      <c r="B6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A7" s="14"/>
+      <c r="B7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="1:5" ht="14.5">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A6" s="17" t="s">
+      <c r="B8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A9" s="32"/>
+      <c r="B9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A10" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="22">
-        <v>-1.157</v>
-      </c>
-      <c r="C6" s="22">
-        <v>-0.20699999999999999</v>
-      </c>
-      <c r="D6" s="23">
-        <v>-0.70899999999999996</v>
-      </c>
-      <c r="E6" s="23">
-        <v>-0.214</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="24" t="s">
+      <c r="B10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A11" s="32"/>
+      <c r="B11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="D11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="E11" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A12" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A14" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A15" s="32"/>
+      <c r="B15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="26">
-        <v>-1.0669999999999999</v>
-      </c>
-      <c r="C8" s="26">
-        <v>-0.188</v>
-      </c>
-      <c r="D8" s="23">
-        <v>-0.65300000000000002</v>
-      </c>
-      <c r="E8" s="23">
-        <v>-0.19500000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="24" t="s">
+      <c r="D15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A17" s="18"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A18" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A19" s="14"/>
+      <c r="B19" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A20" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A21" s="14"/>
+      <c r="B21" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A22" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A23" s="14"/>
+      <c r="B23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="25" t="s">
+      <c r="E23" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A25" s="14"/>
+      <c r="B25" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A26" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A29" s="14"/>
+      <c r="B29" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A30" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A31" s="14"/>
+      <c r="B31" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A32" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A33" s="14"/>
+      <c r="B33" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A34" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A35" s="14"/>
+      <c r="B35" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A36" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="17"/>
+    </row>
+    <row r="37" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A37" s="18"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20"/>
+    </row>
+    <row r="38" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A38" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A39" s="14"/>
+      <c r="B39" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="26">
-        <v>-0.72399999999999998</v>
-      </c>
-      <c r="C10" s="26">
-        <v>-0.12</v>
-      </c>
-      <c r="D10" s="23">
-        <v>-449</v>
-      </c>
-      <c r="E10" s="23">
-        <v>-0.127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A12" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-    </row>
-    <row r="13" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="20">
-        <v>0.27300000000000002</v>
-      </c>
-      <c r="C14" s="20">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="D14" s="18">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="E14" s="18">
-        <v>5.7000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A18" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="26">
-        <v>0.105</v>
-      </c>
-      <c r="C18" s="26">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="D18" s="23">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="E18" s="23">
-        <v>2.1000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A20" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="26">
-        <v>-0.65500000000000003</v>
-      </c>
-      <c r="C20" s="26">
-        <v>-0.14099999999999999</v>
-      </c>
-      <c r="D20" s="23">
-        <v>-0.39900000000000002</v>
-      </c>
-      <c r="E20" s="23">
-        <v>-0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A21" s="9"/>
-      <c r="B21" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A22" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="26">
-        <v>-1233</v>
-      </c>
-      <c r="C22" s="26">
-        <v>-0.26900000000000002</v>
-      </c>
-      <c r="D22" s="23">
-        <v>-0.755</v>
-      </c>
-      <c r="E22" s="23">
-        <v>-0.26900000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A23" s="9"/>
-      <c r="B23" s="27" t="s">
+      <c r="E39" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A40" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A41" s="14"/>
+      <c r="B41" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A24" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="26">
-        <v>0.45300000000000001</v>
-      </c>
-      <c r="C24" s="26">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="D24" s="23">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="E24" s="23">
-        <v>8.4000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A25" s="9"/>
-      <c r="B25" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A26" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="13"/>
-    </row>
-    <row r="27" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16"/>
-    </row>
-    <row r="28" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A28" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="26">
-        <v>-1.7010000000000001</v>
-      </c>
-      <c r="C28" s="26">
-        <v>-0.39400000000000002</v>
-      </c>
-      <c r="D28" s="23">
-        <v>-1.0529999999999999</v>
-      </c>
-      <c r="E28" s="23">
-        <v>-0.39500000000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A29" s="9"/>
-      <c r="B29" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A30" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="26">
-        <v>-3.9950000000000001</v>
-      </c>
-      <c r="C30" s="26">
-        <v>-0.63800000000000001</v>
-      </c>
-      <c r="D30" s="23">
-        <v>-2.2360000000000002</v>
-      </c>
-      <c r="E30" s="23">
-        <v>-0.63600000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A31" s="9"/>
-      <c r="B31" s="27" t="s">
+      <c r="D41" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A32" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="28">
-        <v>-3.028</v>
-      </c>
-      <c r="C32" s="26">
-        <v>-0.58099999999999996</v>
-      </c>
-      <c r="D32" s="23">
-        <v>-1.782</v>
-      </c>
-      <c r="E32" s="23">
-        <v>-0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A33" s="9"/>
-      <c r="B33" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A34" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="28">
-        <v>-3.5070000000000001</v>
-      </c>
-      <c r="C34" s="26">
-        <v>-0.61499999999999999</v>
-      </c>
-      <c r="D34" s="23">
-        <v>-2.0230000000000001</v>
-      </c>
-      <c r="E34" s="23">
-        <v>-0.61399999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A35" s="9"/>
-      <c r="B35" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="25" t="s">
+    </row>
+    <row r="42" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A42" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="10">
+        <v>-2.5000000000000001E-2</v>
+      </c>
+      <c r="C42" s="10">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="D42" s="7">
+        <v>-1.9E-2</v>
+      </c>
+      <c r="E42" s="7">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A43" s="14"/>
+      <c r="B43" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E35" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A36" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="13"/>
-    </row>
-    <row r="37" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A37" s="14"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="16"/>
-    </row>
-    <row r="38" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A38" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="26">
-        <v>-0.187</v>
-      </c>
-      <c r="C38" s="26">
-        <v>-3.9E-2</v>
-      </c>
-      <c r="D38" s="23">
-        <v>-0.11600000000000001</v>
-      </c>
-      <c r="E38" s="23">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A39" s="9"/>
-      <c r="B39" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A40" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="26">
-        <v>-1.046</v>
-      </c>
-      <c r="C40" s="26">
-        <v>-0.23400000000000001</v>
-      </c>
-      <c r="D40" s="23">
-        <v>-0.65800000000000003</v>
-      </c>
-      <c r="E40" s="23">
-        <v>-0.23899999999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A41" s="9"/>
-      <c r="B41" s="27" t="s">
+      <c r="C43" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E41" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A42" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" s="26">
-        <v>-2.5000000000000001E-2</v>
-      </c>
-      <c r="C42" s="26">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="D42" s="23">
-        <v>-1.9E-2</v>
-      </c>
-      <c r="E42" s="23">
-        <v>-6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A43" s="9"/>
-      <c r="B43" s="27" t="s">
+      <c r="D43" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E43" s="25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:5" ht="14.25" customHeight="1"/>
+      <c r="E43" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A44" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+    </row>
+    <row r="45" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A45" s="27"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+    </row>
     <row r="46" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="47" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:5" ht="14.25" customHeight="1"/>
@@ -2208,12 +2415,15 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:E37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
+  <mergeCells count="25">
+    <mergeCell ref="A44:E45"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
     <mergeCell ref="A4:E5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A28:A29"/>
@@ -2226,13 +2436,13 @@
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:E27"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:E37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>